<commit_message>
trial version 1 - customer
</commit_message>
<xml_diff>
--- a/templates/download/add_customers_template.xlsx
+++ b/templates/download/add_customers_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GenoRx\DOCUME~1\MobaXterm\slash\RemoteFiles\132282_3_48\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GenoRx\DOCUME~1\MobaXterm\slash\RemoteFiles\132282_2_238\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="28800" windowHeight="10810"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>備註</t>
   </si>
@@ -66,10 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* 請勿使用簡稱，需填寫正式全名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*姓</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -183,56 +179,110 @@
   </si>
   <si>
     <t>機構名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>機構</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>國立臺灣大學醫學院附設醫院-健康管理中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LINE ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LINE ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*客戶類別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>會員</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 客戶類別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 必須為已有的類別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>* 請勿使用簡稱，需填寫正式全名
 * 請用"-"連接【機構】與【部門/單位】
-* 只接受[機構]-[部門/單位]格式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>機構</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>國立臺灣大學醫學院附設醫院-健康管理中心</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LINE ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>line_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LINE ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*客戶類別</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>會員</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 客戶類別</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 必須為已有的類別</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer_type</t>
+* 只接受[機構]-[部門/單位]格式
+* 必須為已有機構</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 請勿使用簡稱，需填寫正式全名
+* 必須為已有職業</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 請勿使用簡稱，需填寫正式全名
+* 必須為已有職稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>毛茸茸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推薦人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關係</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配偶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relationship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推薦人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關係</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 必須為已有的關係
+* 若有填寫此欄，則必填【推薦人】</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 必須為已有的客戶
+* 若有填寫此欄，則必填【關係】
+* 若有同名客戶，請使用【新增客戶】新增此客戶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>introducer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -776,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -795,9 +845,11 @@
     <col min="10" max="10" width="18.54296875" style="1" customWidth="1"/>
     <col min="11" max="11" width="17.6328125" style="1" customWidth="1"/>
     <col min="12" max="13" width="20.36328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" customWidth="1"/>
+    <col min="15" max="15" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="69.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="69.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -805,51 +857,57 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="L2" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="102" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="119" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -859,29 +917,35 @@
         <v>7</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" s="15"/>
       <c r="M3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" ht="34" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -895,121 +959,139 @@
         <v>32195</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="K4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="L4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="M4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" s="24"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="28" t="s">
+      <c r="F5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="27" t="s">
+      <c r="G5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="H5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="27" t="s">
+      <c r="J5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="K5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="L5" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="M5" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="19" t="s">
+      <c r="G6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="19" t="s">
+      <c r="K6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="19" t="s">
-        <v>16</v>
-      </c>
       <c r="L6" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="N6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1025,7 +1107,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1041,7 +1123,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1057,7 +1139,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1073,7 +1155,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1089,7 +1171,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1105,7 +1187,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1121,7 +1203,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1137,7 +1219,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>

</xml_diff>